<commit_message>
plotting with kenyan map
</commit_message>
<xml_diff>
--- a/contacts/session_params.xlsx
+++ b/contacts/session_params.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" tabRatio="583"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" tabRatio="583" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ContactTracing_v3" sheetId="1" r:id="rId1"/>
+    <sheet name="ContactTracing_v4" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="102">
   <si>
     <t>tau p</t>
   </si>
@@ -1944,6 +1945,91 @@
     <t>atom PERMISSION DENIED
 done</t>
   </si>
+  <si>
+    <t>[0.0,0.25,0.5,0.75,0.9]</t>
+  </si>
+  <si>
+    <t>τₚ_list</t>
+  </si>
+  <si>
+    <t>session num</t>
+  </si>
+  <si>
+    <t>1/3.</t>
+  </si>
+  <si>
+    <t>κₘ=Δₜ 
+(memory and tracing period)</t>
+  </si>
+  <si>
+    <t>P.κ 
+(mean nb contacts/day)</t>
+  </si>
+  <si>
+    <t>Κ_max_capacity 
+(tracing capacity)</t>
+  </si>
+  <si>
+    <t>P.τ 
+(detection rate)</t>
+  </si>
+  <si>
+    <t>P.κ_per_event4</t>
+  </si>
+  <si>
+    <t>Nairobi=1e3</t>
+  </si>
+  <si>
+    <t>Nairobi=1e3
+Mombassa=1e3</t>
+  </si>
+  <si>
+    <t>Nairobi=1e3
+Mombassa=1e3
+All others = 1e2</t>
+  </si>
+  <si>
+    <t>n_traj</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>Session20 Running 200 sims for τₚ=0.0
+322.019146 seconds (5.29 G allocations: 117.243 GiB, 4.94% gc time)
+Session20 Running 200 sims for τₚ=0.25
+417.853990 seconds (6.70 G allocations: 164.213 GiB, 9.38% gc time)
+Session20 Running 200 sims for τₚ=0.5
+465.380005 seconds (6.62 G allocations: 161.609 GiB, 17.32% gc time)
+Session20 Running 200 sims for τₚ=0.75
+449.716149 seconds (6.53 G allocations: 158.466 GiB, 17.67% gc time)
+Session20 Running 200 sims for τₚ=0.9
+456.834434 seconds (6.51 G allocations: 158.014 GiB, 17.94% gc time)</t>
+  </si>
+  <si>
+    <t>Session21 Running 200 sims for τₚ=0.0
+335.654335 seconds (5.29 G allocations: 117.288 GiB, 5.23% gc time)
+Session21 Running 200 sims for τₚ=0.25
+465.765592 seconds (7.37 G allocations: 194.208 GiB, 10.84% gc time)
+Session21 Running 200 sims for τₚ=0.5
+495.388642 seconds (7.28 G allocations: 191.140 GiB, 19.02% gc time)
+Session21 Running 200 sims for τₚ=0.75
+497.745998 seconds (7.26 G allocations: 190.629 GiB, 18.27% gc time)
+Session21 Running 200 sims for τₚ=0.9
+493.368206 seconds (7.23 G allocations: 189.397 GiB, 18.97% gc time)</t>
+  </si>
+  <si>
+    <t>Session22 Running 200 sims for τₚ=0.0
+408.752327 seconds (5.27 G allocations: 116.212 GiB, 23.90% gc time)
+Session22 Running 200 sims for τₚ=0.25
+589.263548 seconds (11.32 G allocations: 355.409 GiB, 18.57% gc time)
+Session22 Running 200 sims for τₚ=0.5
+705.803741 seconds (11.97 G allocations: 384.555 GiB, 25.88% gc time)
+Session22 Running 200 sims for τₚ=0.75
+789.517263 seconds (11.64 G allocations: 376.236 GiB, 30.35% gc time)
+Session22 Running 200 sims for τₚ=0.9
+764.713482 seconds (11.26 G allocations: 361.700 GiB, 29.63% gc time)</t>
+  </si>
 </sst>
 </file>
 
@@ -2028,7 +2114,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2091,6 +2177,39 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2907,9 +3026,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H31" sqref="H31"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3791,4 +3910,254 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K4" sqref="K4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="49.85546875" style="33" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="27" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="26"/>
+    </row>
+    <row r="2" spans="1:11" s="28" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="28">
+        <v>10</v>
+      </c>
+      <c r="D2" s="28">
+        <v>7</v>
+      </c>
+      <c r="E2" s="28">
+        <v>50</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="G2" s="28">
+        <v>200</v>
+      </c>
+      <c r="H2" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="28">
+        <v>20</v>
+      </c>
+      <c r="J2" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="K2" s="30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="28" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="F3" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="28">
+        <v>21</v>
+      </c>
+      <c r="J3" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="K3" s="30" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="28" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="F4" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="H4" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="28">
+        <v>22</v>
+      </c>
+      <c r="J4" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="K4" s="30" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I5" s="28">
+        <v>23</v>
+      </c>
+      <c r="K5" s="31"/>
+    </row>
+    <row r="6" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I6" s="28">
+        <v>24</v>
+      </c>
+      <c r="K6" s="31"/>
+    </row>
+    <row r="7" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="28">
+        <v>25</v>
+      </c>
+      <c r="K7" s="31"/>
+    </row>
+    <row r="8" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K8" s="31"/>
+    </row>
+    <row r="9" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K9" s="31"/>
+    </row>
+    <row r="10" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K10" s="31"/>
+    </row>
+    <row r="11" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K11" s="31"/>
+    </row>
+    <row r="12" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K12" s="31"/>
+    </row>
+    <row r="13" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K13" s="31"/>
+    </row>
+    <row r="14" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K14" s="31"/>
+    </row>
+    <row r="15" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K15" s="31"/>
+    </row>
+    <row r="16" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K16" s="31"/>
+    </row>
+    <row r="17" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K17" s="31"/>
+    </row>
+    <row r="18" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K18" s="31"/>
+    </row>
+    <row r="19" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K19" s="31"/>
+    </row>
+    <row r="20" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K20" s="31"/>
+    </row>
+    <row r="21" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K21" s="31"/>
+    </row>
+    <row r="22" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K22" s="31"/>
+    </row>
+    <row r="23" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K23" s="31"/>
+    </row>
+    <row r="24" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K24" s="31"/>
+    </row>
+    <row r="25" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K25" s="31"/>
+    </row>
+    <row r="26" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K26" s="31"/>
+    </row>
+    <row r="27" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K27" s="31"/>
+    </row>
+    <row r="28" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K28" s="31"/>
+    </row>
+    <row r="29" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K29" s="31"/>
+    </row>
+    <row r="30" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K30" s="31"/>
+    </row>
+    <row r="31" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K31" s="31"/>
+    </row>
+    <row r="32" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K32" s="31"/>
+    </row>
+    <row r="33" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K33" s="31"/>
+    </row>
+    <row r="34" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K34" s="31"/>
+    </row>
+    <row r="35" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K35" s="32"/>
+    </row>
+    <row r="36" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K36" s="32"/>
+    </row>
+    <row r="37" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K37" s="32"/>
+    </row>
+    <row r="38" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K38" s="32"/>
+    </row>
+    <row r="39" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K39" s="32"/>
+    </row>
+    <row r="40" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K40" s="32"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Event 4 IQ->Q uses a rate and not a duration
-Event 4 IQ->Q is no longer done with duration 1/tau, but using the rate tau (like all other events
-Contact.detection_dur is no longer used (to be deleted)
</commit_message>
<xml_diff>
--- a/contacts/session_params.xlsx
+++ b/contacts/session_params.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\marlon.ads.warwick.ac.uk\User56\u\u1875687\Desktop\RabiaGitHub\KenyaCoV\contacts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rabia\Documents\GitHub\KenyaCoV\contacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12336" tabRatio="583" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" tabRatio="583" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ContactTracing_v3" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="106">
   <si>
     <t>tau p</t>
   </si>
@@ -2096,7 +2096,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2127,6 +2127,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2140,7 +2146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2236,6 +2242,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3057,22 +3069,22 @@
       <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.44140625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.88671875" style="7" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.5546875" style="7" customWidth="1"/>
-    <col min="9" max="9" width="77.88671875" style="9" customWidth="1"/>
-    <col min="10" max="10" width="57.109375" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="2"/>
+    <col min="1" max="1" width="8.42578125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" style="7" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="77.85546875" style="9" customWidth="1"/>
+    <col min="10" max="10" width="57.140625" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3099,7 +3111,7 @@
       </c>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:9" ht="102" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="105" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>0</v>
       </c>
@@ -3128,7 +3140,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="102" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="105" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>0.05</v>
       </c>
@@ -3157,7 +3169,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="102" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="105" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>0.05</v>
       </c>
@@ -3186,7 +3198,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="102" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="105" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>0.05</v>
       </c>
@@ -3215,7 +3227,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="102" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="105" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>0.1</v>
       </c>
@@ -3244,7 +3256,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="102" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="105" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>0.1</v>
       </c>
@@ -3273,7 +3285,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="102" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="105" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>0.1</v>
       </c>
@@ -3302,7 +3314,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D9" s="7" t="s">
         <v>56</v>
       </c>
@@ -3310,7 +3322,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D10" s="7" t="s">
         <v>56</v>
       </c>
@@ -3318,7 +3330,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="115.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>0.3</v>
       </c>
@@ -3347,7 +3359,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="100.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>0.3</v>
       </c>
@@ -3376,7 +3388,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="99.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
         <v>0.3</v>
       </c>
@@ -3405,7 +3417,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="99" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="99" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="11">
         <v>0.5</v>
       </c>
@@ -3434,7 +3446,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="11">
         <v>0.5</v>
       </c>
@@ -3463,7 +3475,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
         <v>0.5</v>
       </c>
@@ -3480,7 +3492,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="107.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="19">
         <v>0.8</v>
       </c>
@@ -3509,7 +3521,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="106.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="19">
         <v>0.8</v>
       </c>
@@ -3538,7 +3550,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="19">
         <v>0.8</v>
       </c>
@@ -3564,19 +3576,19 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="5">
         <v>0.05</v>
       </c>
@@ -3602,7 +3614,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="5">
         <v>0.1</v>
       </c>
@@ -3628,7 +3640,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="106.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="5">
         <v>0.05</v>
       </c>
@@ -3657,7 +3669,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="186.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="186.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
         <v>0.1</v>
       </c>
@@ -3686,7 +3698,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="115.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
         <v>0.2</v>
       </c>
@@ -3715,7 +3727,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="161.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="161.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="5">
         <v>0.3</v>
       </c>
@@ -3744,7 +3756,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="147.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5">
         <v>0.4</v>
       </c>
@@ -3771,7 +3783,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="153.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="153.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5">
         <v>0.5</v>
       </c>
@@ -3798,7 +3810,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="159" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="159" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5">
         <v>0.6</v>
       </c>
@@ -3825,7 +3837,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="161.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="161.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="5">
         <v>0.7</v>
       </c>
@@ -3852,7 +3864,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="161.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="161.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="5">
         <v>0.8</v>
       </c>
@@ -3881,52 +3893,52 @@
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B44" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B46" s="7" t="s">
         <v>27</v>
       </c>
@@ -3942,28 +3954,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="49.88671875" style="33" customWidth="1"/>
-    <col min="12" max="16384" width="9.109375" style="2"/>
+    <col min="8" max="8" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="49.85546875" style="33" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="27" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="27" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
         <v>86</v>
       </c>
@@ -3996,7 +4008,7 @@
       </c>
       <c r="K1" s="26"/>
     </row>
-    <row r="2" spans="1:11" s="28" customFormat="1" ht="102" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" s="28" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>85</v>
       </c>
@@ -4031,7 +4043,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="28" customFormat="1" ht="102" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" s="28" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="F3" s="29" t="s">
         <v>95</v>
       </c>
@@ -4048,7 +4060,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="28" customFormat="1" ht="102" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" s="28" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="F4" s="29" t="s">
         <v>96</v>
       </c>
@@ -4065,16 +4077,16 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K5" s="31"/>
     </row>
-    <row r="6" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K6" s="31"/>
     </row>
-    <row r="7" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K7" s="31"/>
     </row>
-    <row r="8" spans="1:11" s="28" customFormat="1" ht="176.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" s="28" customFormat="1" ht="176.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
         <v>102</v>
       </c>
@@ -4103,10 +4115,10 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K9" s="31"/>
     </row>
-    <row r="10" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
         <v>85</v>
       </c>
@@ -4133,106 +4145,157 @@
       </c>
       <c r="K10" s="31"/>
     </row>
-    <row r="11" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="G11" s="28">
+    <row r="11" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" s="34">
+        <v>10</v>
+      </c>
+      <c r="D11" s="34">
+        <v>7</v>
+      </c>
+      <c r="E11" s="34">
+        <v>50</v>
+      </c>
+      <c r="F11" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="G11" s="34">
         <v>100</v>
       </c>
-      <c r="I11" s="28">
+      <c r="H11" s="34"/>
+      <c r="I11" s="34">
         <v>36</v>
       </c>
       <c r="K11" s="31"/>
     </row>
-    <row r="12" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F12" s="28" t="s">
+    <row r="12" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" s="34">
+        <v>10</v>
+      </c>
+      <c r="D12" s="34">
+        <v>7</v>
+      </c>
+      <c r="E12" s="34">
+        <v>50</v>
+      </c>
+      <c r="F12" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="G12" s="28">
+      <c r="G12" s="34">
         <v>100</v>
       </c>
-      <c r="I12" s="28">
+      <c r="H12" s="34"/>
+      <c r="I12" s="34">
         <v>37</v>
       </c>
       <c r="K12" s="31"/>
     </row>
-    <row r="13" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F13" s="28" t="s">
+    <row r="13" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" s="34">
+        <v>10</v>
+      </c>
+      <c r="D13" s="34">
+        <v>7</v>
+      </c>
+      <c r="E13" s="34">
+        <v>50</v>
+      </c>
+      <c r="F13" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="G13" s="28">
+      <c r="G13" s="34">
         <v>100</v>
       </c>
-      <c r="I13" s="28">
+      <c r="H13" s="34"/>
+      <c r="I13" s="34">
         <v>38</v>
       </c>
       <c r="K13" s="31"/>
     </row>
-    <row r="14" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K14" s="31"/>
     </row>
-    <row r="15" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K15" s="31"/>
     </row>
-    <row r="16" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K16" s="31"/>
     </row>
-    <row r="17" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K17" s="31"/>
     </row>
-    <row r="18" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K18" s="31"/>
     </row>
-    <row r="19" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K19" s="31"/>
     </row>
-    <row r="20" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K20" s="31"/>
     </row>
-    <row r="21" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K21" s="31"/>
     </row>
-    <row r="22" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K22" s="31"/>
     </row>
-    <row r="23" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K23" s="31"/>
     </row>
-    <row r="24" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K24" s="31"/>
     </row>
-    <row r="25" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K25" s="31"/>
     </row>
-    <row r="26" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K26" s="31"/>
     </row>
-    <row r="27" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K27" s="31"/>
     </row>
-    <row r="28" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K28" s="31"/>
     </row>
-    <row r="29" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K29" s="31"/>
     </row>
-    <row r="30" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K30" s="31"/>
     </row>
-    <row r="31" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K31" s="32"/>
     </row>
-    <row r="32" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K32" s="32"/>
     </row>
-    <row r="33" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K33" s="32"/>
     </row>
-    <row r="34" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K34" s="32"/>
     </row>
-    <row r="35" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K35" s="32"/>
     </row>
-    <row r="36" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K36" s="32"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Kilifi results sent to team
- removed state 11 C (contacts)
- added state 11 Qs = quarantined susceptibles
- added p.Q_dur = duration of quarantine
- added event 16 Qs->S with rate 1/p.Q_dur
- use output function output_daily_and_final_incidence
</commit_message>
<xml_diff>
--- a/contacts/session_params.xlsx
+++ b/contacts/session_params.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="118">
   <si>
     <t>tau p</t>
   </si>
@@ -2354,6 +2354,31 @@
 2501.999148 seconds (26.90 G allocations: 894.665 GiB, 48.36% gc time)
 Session44 Running 200 sims for τₚ=0.75</t>
   </si>
+  <si>
+    <t>Session55 Running 100 sims for τₚ=0.0
+Session55 Running 100 sims for τₚ=0.25
+Session55 Running 100 sims for τₚ=0.5
+Session55 Running 100 sims for τₚ=0.75
+Session55 Running 100 sims for τₚ=0.9</t>
+  </si>
+  <si>
+    <t>Session56 Running 100 sims for τₚ=0.0
+Session56 Running 100 sims for τₚ=0.25
+Session56 Running 100 sims for τₚ=0.5
+Session56 Running 100 sims for τₚ=0.75
+Session56 Running 100 sims for τₚ=0.9
+4515.861133 seconds (63.73 G allocations: 2.537 TiB, 61.37% gc time)</t>
+  </si>
+  <si>
+    <t>WITH S AND R</t>
+  </si>
+  <si>
+    <t>Session57 Running 100 sims for τₚ=0.25
+Session57 Running 100 sims for τₚ=0.5
+Session57 Running 100 sims for τₚ=0.75
+Session57 Running 100 sims for τₚ=0.9
+4175.755049 seconds (164.58 G allocations: 5.928 TiB, 44.46% gc time)</t>
+  </si>
 </sst>
 </file>
 
@@ -2394,7 +2419,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2445,13 +2470,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2468,7 +2499,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2591,6 +2622,13 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4295,11 +4333,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I39" sqref="A39:I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4679,19 +4717,19 @@
       </c>
     </row>
     <row r="20" spans="1:11" s="28" customFormat="1" ht="52.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="42"/>
-      <c r="B20" s="42"/>
-      <c r="C20" s="42"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="42" t="s">
+      <c r="A20" s="41"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="G20" s="42">
+      <c r="G20" s="41">
         <v>200</v>
       </c>
-      <c r="H20" s="42"/>
-      <c r="I20" s="42">
+      <c r="H20" s="41"/>
+      <c r="I20" s="41">
         <v>44</v>
       </c>
       <c r="K20" s="30" t="s">
@@ -4699,19 +4737,19 @@
       </c>
     </row>
     <row r="21" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="42"/>
-      <c r="B21" s="42"/>
-      <c r="C21" s="42"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42" t="s">
+      <c r="A21" s="41"/>
+      <c r="B21" s="41"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="G21" s="42">
+      <c r="G21" s="41">
         <v>200</v>
       </c>
-      <c r="H21" s="42"/>
-      <c r="I21" s="42">
+      <c r="H21" s="41"/>
+      <c r="I21" s="41">
         <v>45</v>
       </c>
       <c r="K21" s="31"/>
@@ -4723,65 +4761,50 @@
       <c r="K23" s="31"/>
     </row>
     <row r="24" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="41" t="s">
-        <v>85</v>
-      </c>
-      <c r="B24" s="41" t="s">
-        <v>88</v>
-      </c>
-      <c r="C24" s="41">
-        <v>10</v>
-      </c>
-      <c r="D24" s="41">
-        <v>7</v>
-      </c>
-      <c r="E24" s="41">
-        <v>50</v>
-      </c>
-      <c r="F24" s="41" t="s">
+      <c r="F24" s="42" t="s">
         <v>106</v>
       </c>
-      <c r="G24" s="41">
+      <c r="G24" s="42">
         <v>500</v>
       </c>
-      <c r="H24" s="41"/>
-      <c r="I24" s="41">
+      <c r="H24" s="42"/>
+      <c r="I24" s="42">
         <v>46</v>
       </c>
       <c r="K24" s="31"/>
     </row>
     <row r="25" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="41"/>
-      <c r="B25" s="41"/>
-      <c r="C25" s="41"/>
-      <c r="D25" s="41"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="41" t="s">
+      <c r="A25" s="42"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="G25" s="41">
+      <c r="G25" s="42">
         <v>500</v>
       </c>
-      <c r="H25" s="41"/>
-      <c r="I25" s="41">
+      <c r="H25" s="42"/>
+      <c r="I25" s="42">
         <v>47</v>
       </c>
       <c r="K25" s="31"/>
     </row>
     <row r="26" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="41"/>
-      <c r="B26" s="41"/>
-      <c r="C26" s="41"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="41"/>
-      <c r="F26" s="41" t="s">
+      <c r="A26" s="42"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42" t="s">
         <v>107</v>
       </c>
-      <c r="G26" s="41">
+      <c r="G26" s="42">
         <v>500</v>
       </c>
-      <c r="H26" s="41"/>
-      <c r="I26" s="41">
+      <c r="H26" s="42"/>
+      <c r="I26" s="42">
         <v>48</v>
       </c>
       <c r="K26" s="31"/>
@@ -4793,28 +4816,306 @@
       <c r="K28" s="31"/>
     </row>
     <row r="29" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="K29" s="31"/>
+      <c r="A29" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="B29" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29" s="36">
+        <v>10</v>
+      </c>
+      <c r="D29" s="36">
+        <v>7</v>
+      </c>
+      <c r="E29" s="36">
+        <v>50</v>
+      </c>
+      <c r="F29" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="G29" s="36">
+        <v>10</v>
+      </c>
+      <c r="H29" s="36"/>
+      <c r="I29" s="36">
+        <v>51</v>
+      </c>
+      <c r="K29" s="31" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="30" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="K30" s="31"/>
+      <c r="A30" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" s="37">
+        <v>10</v>
+      </c>
+      <c r="D30" s="37">
+        <v>7</v>
+      </c>
+      <c r="E30" s="37">
+        <v>50</v>
+      </c>
+      <c r="F30" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="G30" s="37">
+        <v>10</v>
+      </c>
+      <c r="H30" s="37"/>
+      <c r="I30" s="37">
+        <v>52</v>
+      </c>
+      <c r="K30" s="31" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="31" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="K31" s="32"/>
+      <c r="A31" s="36"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="36"/>
+      <c r="E31" s="36"/>
+      <c r="F31" s="36" t="s">
+        <v>107</v>
+      </c>
+      <c r="G31" s="36">
+        <v>10</v>
+      </c>
+      <c r="H31" s="36"/>
+      <c r="I31" s="36">
+        <v>53</v>
+      </c>
+      <c r="K31" s="31" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="32" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="K32" s="32"/>
-    </row>
-    <row r="33" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="K33" s="32"/>
-    </row>
-    <row r="34" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="K34" s="32"/>
-    </row>
-    <row r="35" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="K35" s="32"/>
-    </row>
-    <row r="36" spans="11:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="K36" s="32"/>
+      <c r="K32" s="31"/>
+    </row>
+    <row r="33" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K33" s="31"/>
+    </row>
+    <row r="34" spans="1:11" s="28" customFormat="1" ht="52.5" x14ac:dyDescent="0.25">
+      <c r="A34" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="B34" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="C34" s="36">
+        <v>10</v>
+      </c>
+      <c r="D34" s="36">
+        <v>7</v>
+      </c>
+      <c r="E34" s="36">
+        <v>50</v>
+      </c>
+      <c r="F34" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="G34" s="36">
+        <v>100</v>
+      </c>
+      <c r="H34" s="36"/>
+      <c r="I34" s="36">
+        <v>55</v>
+      </c>
+      <c r="K34" s="30" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" s="28" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A35" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="C35" s="37">
+        <v>10</v>
+      </c>
+      <c r="D35" s="37">
+        <v>7</v>
+      </c>
+      <c r="E35" s="37">
+        <v>50</v>
+      </c>
+      <c r="F35" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="G35" s="37">
+        <v>100</v>
+      </c>
+      <c r="H35" s="37"/>
+      <c r="I35" s="37">
+        <v>56</v>
+      </c>
+      <c r="K35" s="30" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" s="28" customFormat="1" ht="52.5" x14ac:dyDescent="0.25">
+      <c r="A36" s="36"/>
+      <c r="B36" s="36"/>
+      <c r="C36" s="36"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36" t="s">
+        <v>107</v>
+      </c>
+      <c r="G36" s="36"/>
+      <c r="H36" s="36"/>
+      <c r="I36" s="36">
+        <v>57</v>
+      </c>
+      <c r="K36" s="30" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K37" s="32"/>
+    </row>
+    <row r="38" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K38" s="32"/>
+    </row>
+    <row r="39" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="C39" s="43">
+        <v>10</v>
+      </c>
+      <c r="D39" s="43">
+        <v>7</v>
+      </c>
+      <c r="E39" s="43">
+        <v>50</v>
+      </c>
+      <c r="F39" s="43" t="s">
+        <v>106</v>
+      </c>
+      <c r="G39" s="43">
+        <v>1000</v>
+      </c>
+      <c r="H39" s="43"/>
+      <c r="I39" s="43">
+        <v>60</v>
+      </c>
+      <c r="K39" s="32"/>
+    </row>
+    <row r="40" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="43"/>
+      <c r="B40" s="43"/>
+      <c r="C40" s="43"/>
+      <c r="D40" s="43"/>
+      <c r="E40" s="43"/>
+      <c r="F40" s="43" t="s">
+        <v>108</v>
+      </c>
+      <c r="G40" s="43">
+        <v>1000</v>
+      </c>
+      <c r="H40" s="43"/>
+      <c r="I40" s="43">
+        <v>61</v>
+      </c>
+      <c r="K40" s="32"/>
+    </row>
+    <row r="41" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="43"/>
+      <c r="B41" s="43"/>
+      <c r="C41" s="43"/>
+      <c r="D41" s="43"/>
+      <c r="E41" s="43"/>
+      <c r="F41" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="G41" s="43">
+        <v>1000</v>
+      </c>
+      <c r="H41" s="43"/>
+      <c r="I41" s="43">
+        <v>62</v>
+      </c>
+      <c r="K41" s="32"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A42" s="44"/>
+      <c r="B42" s="44"/>
+      <c r="C42" s="44"/>
+      <c r="D42" s="44"/>
+      <c r="E42" s="44"/>
+      <c r="F42" s="44"/>
+      <c r="G42" s="44"/>
+      <c r="H42" s="44"/>
+      <c r="I42" s="44"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43" s="45"/>
+      <c r="B43" s="45"/>
+      <c r="C43" s="45"/>
+      <c r="D43" s="45"/>
+      <c r="E43" s="45">
+        <v>100</v>
+      </c>
+      <c r="F43" s="43" t="s">
+        <v>106</v>
+      </c>
+      <c r="G43" s="43">
+        <v>1000</v>
+      </c>
+      <c r="H43" s="45"/>
+      <c r="I43" s="45">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A44" s="45"/>
+      <c r="B44" s="45"/>
+      <c r="C44" s="45"/>
+      <c r="D44" s="45"/>
+      <c r="E44" s="45">
+        <v>100</v>
+      </c>
+      <c r="F44" s="43" t="s">
+        <v>108</v>
+      </c>
+      <c r="G44" s="45">
+        <v>1000</v>
+      </c>
+      <c r="H44" s="45"/>
+      <c r="I44" s="45">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A45" s="45"/>
+      <c r="B45" s="45"/>
+      <c r="C45" s="45"/>
+      <c r="D45" s="45"/>
+      <c r="E45" s="45">
+        <v>100</v>
+      </c>
+      <c r="F45" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="G45" s="45">
+        <v>1000</v>
+      </c>
+      <c r="H45" s="45"/>
+      <c r="I45" s="45">
+        <v>67</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>